<commit_message>
Actualizar archivos de base de datos y datos de Excel
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/MC2020moded.xlsx
+++ b/quickshift/src/datafiles/MC2020moded.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="9540" windowHeight="12420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MallaCurricular2020" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Electivos" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equivalencias" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MallaCurricular2020" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Electivos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Equivalencias" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -2969,16 +2969,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>CIG1014</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>CIG1003</t>
-        </is>
-      </c>
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="6" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">

</xml_diff>

<commit_message>
feat: actualizar archivos de base de datos y hojas de cálculo para mejorar el análisis
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/MC2020moded.xlsx
+++ b/quickshift/src/datafiles/MC2020moded.xlsx
@@ -2928,107 +2928,51 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.141666666666669" defaultRowHeight="15"/>
-  <cols>
-    <col width="37.2833333333333" customWidth="1" min="1" max="1"/>
-    <col width="49.5666666666667" customWidth="1" min="2" max="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Código Antiguo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Código Nuevo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CIG1012</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CIG1003</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>CIG1013</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>CIG1003</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>CIG1012</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>CIG1002</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="n"/>
-      <c r="B4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>